<commit_message>
Removing excess code to smooth marge with esp-32
</commit_message>
<xml_diff>
--- a/macierze_numeryczne_Ai.xlsx
+++ b/macierze_numeryczne_Ai.xlsx
@@ -428,30 +428,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B1" t="n">
-        <v>-7.498798913309288e-33</v>
+        <v>0</v>
       </c>
       <c r="C1" t="n">
-        <v>1.224646799147353e-16</v>
+        <v>0</v>
       </c>
       <c r="D1" t="n">
-        <v>-18.4</v>
+        <v>18.4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1.224646799147353e-16</v>
+        <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>-6.123233995736766e-17</v>
+        <v>6.123233995736766e-17</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D2" t="n">
-        <v>2.25335011043113e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -503,30 +503,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>0.8731594033696064</v>
+        <v>1</v>
       </c>
       <c r="B1" t="n">
-        <v>-0.4874347713358506</v>
+        <v>0</v>
       </c>
       <c r="C1" t="n">
         <v>0</v>
       </c>
       <c r="D1" t="n">
-        <v>130.1007511020713</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.4874347713358506</v>
+        <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.8731594033696064</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>72.62778092904173</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -578,30 +578,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>0.6545168930638546</v>
+        <v>1</v>
       </c>
       <c r="B1" t="n">
-        <v>-0.7560473772813703</v>
+        <v>0</v>
       </c>
       <c r="C1" t="n">
         <v>0</v>
       </c>
       <c r="D1" t="n">
-        <v>78.73838223558171</v>
+        <v>120.3</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.7560473772813703</v>
+        <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.6545168930638546</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>90.95249948694884</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -653,30 +653,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>0.548863615966837</v>
+        <v>6.123233995736766e-17</v>
       </c>
       <c r="B1" t="n">
-        <v>-5.118484260602706e-17</v>
+        <v>6.123233995736766e-17</v>
       </c>
       <c r="C1" t="n">
-        <v>-0.8359119158546602</v>
+        <v>1</v>
       </c>
       <c r="D1" t="n">
-        <v>48.19022548188828</v>
+        <v>5.37619944825688e-15</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.8359119158546602</v>
+        <v>-1</v>
       </c>
       <c r="B2" t="n">
-        <v>3.360820352311145e-17</v>
+        <v>3.749399456654644e-33</v>
       </c>
       <c r="C2" t="n">
-        <v>0.548863615966837</v>
+        <v>6.123233995736766e-17</v>
       </c>
       <c r="D2" t="n">
-        <v>73.39306621203916</v>
+        <v>-87.8</v>
       </c>
     </row>
     <row r="3">
@@ -803,44 +803,44 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>0.7071067811865475</v>
+        <v>6.123233995736766e-17</v>
       </c>
       <c r="B1" t="n">
-        <v>-7.916687710296066e-17</v>
+        <v>6.123233995736766e-17</v>
       </c>
       <c r="C1" t="n">
-        <v>0.7071067811865475</v>
+        <v>1</v>
       </c>
       <c r="D1" t="n">
-        <v>-87.49999999999999</v>
+        <v>297.7</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-1.29893408435324e-16</v>
+        <v>-6.123233995736766e-17</v>
       </c>
       <c r="B2" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>1.793453714559298e-17</v>
+        <v>-6.123233995736766e-17</v>
       </c>
       <c r="D2" t="n">
-        <v>-4.696520474730098e-15</v>
+        <v>-7.396866666850013e-15</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.7071067811865475</v>
+        <v>-1</v>
       </c>
       <c r="B3" t="n">
-        <v>-1.045301427691423e-16</v>
+        <v>-6.123233995736766e-17</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.7071067811865475</v>
+        <v>6.123233995736766e-17</v>
       </c>
       <c r="D3" t="n">
-        <v>372.4999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">

</xml_diff>